<commit_message>
Code updated 22-12-30 14:26:46
</commit_message>
<xml_diff>
--- a/Season_Attack/80.xlsx
+++ b/Season_Attack/80.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y174"/>
+  <dimension ref="A1:AA175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,16 @@
           <t>12-28_0</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>12-29_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>12-29_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -596,9 +606,15 @@
       <c r="X2" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>3560</t>
+      <c r="Y2" t="n">
+        <v>3560</v>
+      </c>
+      <c r="Z2" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>3895</t>
         </is>
       </c>
     </row>
@@ -681,9 +697,15 @@
       <c r="X3" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>4870</t>
+      <c r="Y3" t="n">
+        <v>4870</v>
+      </c>
+      <c r="Z3" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>5259</t>
         </is>
       </c>
     </row>
@@ -766,7 +788,13 @@
       <c r="X4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Y4" t="n">
+        <v>4491</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>4491</t>
         </is>
@@ -851,9 +879,15 @@
       <c r="X5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>5814</t>
+      <c r="Y5" t="n">
+        <v>5814</v>
+      </c>
+      <c r="Z5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>6125</t>
         </is>
       </c>
     </row>
@@ -936,9 +970,15 @@
       <c r="X6" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>5889</t>
+      <c r="Y6" t="n">
+        <v>5889</v>
+      </c>
+      <c r="Z6" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>6192</t>
         </is>
       </c>
     </row>
@@ -1021,9 +1061,15 @@
       <c r="X7" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>5975</t>
+      <c r="Y7" t="n">
+        <v>5975</v>
+      </c>
+      <c r="Z7" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>6234</t>
         </is>
       </c>
     </row>
@@ -1106,9 +1152,15 @@
       <c r="X8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>5208</t>
+      <c r="Y8" t="n">
+        <v>5208</v>
+      </c>
+      <c r="Z8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>5436</t>
         </is>
       </c>
     </row>
@@ -1191,9 +1243,15 @@
       <c r="X9" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>5420</t>
+      <c r="Y9" t="n">
+        <v>5420</v>
+      </c>
+      <c r="Z9" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>5598</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1274,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F10" s="5" t="n">
@@ -1276,9 +1334,15 @@
       <c r="X10" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>5598</t>
+      <c r="Y10" t="n">
+        <v>5598</v>
+      </c>
+      <c r="Z10" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>5720</t>
         </is>
       </c>
     </row>
@@ -1361,9 +1425,15 @@
       <c r="X11" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>6398</t>
+      <c r="Y11" t="n">
+        <v>6398</v>
+      </c>
+      <c r="Z11" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>6739</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1456,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F12" s="3" t="n">
@@ -1446,9 +1516,15 @@
       <c r="X12" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>5271</t>
+      <c r="Y12" t="n">
+        <v>5271</v>
+      </c>
+      <c r="Z12" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>5463</t>
         </is>
       </c>
     </row>
@@ -1531,9 +1607,15 @@
       <c r="X13" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>5102</t>
+      <c r="Y13" t="n">
+        <v>5102</v>
+      </c>
+      <c r="Z13" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>5341</t>
         </is>
       </c>
     </row>
@@ -1556,7 +1638,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F14" s="5" t="n">
@@ -1616,9 +1698,15 @@
       <c r="X14" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>6153</t>
+      <c r="Y14" t="n">
+        <v>6153</v>
+      </c>
+      <c r="Z14" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>6327</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1729,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F15" s="3" t="n">
@@ -1701,9 +1789,15 @@
       <c r="X15" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="Y15" t="n">
+        <v>5334</v>
+      </c>
+      <c r="Z15" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>5432</t>
         </is>
       </c>
     </row>
@@ -1786,9 +1880,15 @@
       <c r="X16" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>5977</t>
+      <c r="Y16" t="n">
+        <v>5977</v>
+      </c>
+      <c r="Z16" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>6306</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1911,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F17" s="3" t="n">
@@ -1871,9 +1971,15 @@
       <c r="X17" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>5407</t>
+      <c r="Y17" t="n">
+        <v>5407</v>
+      </c>
+      <c r="Z17" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>5609</t>
         </is>
       </c>
     </row>
@@ -1956,9 +2062,15 @@
       <c r="X18" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>5007</t>
+      <c r="Y18" t="n">
+        <v>5007</v>
+      </c>
+      <c r="Z18" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>5159</t>
         </is>
       </c>
     </row>
@@ -2041,9 +2153,15 @@
       <c r="X19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>5805</t>
+      <c r="Y19" t="n">
+        <v>5805</v>
+      </c>
+      <c r="Z19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>5957</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2244,15 @@
       <c r="X20" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>5673</t>
+      <c r="Y20" t="n">
+        <v>5673</v>
+      </c>
+      <c r="Z20" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>5805</t>
         </is>
       </c>
     </row>
@@ -2211,9 +2335,15 @@
       <c r="X21" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>4885</t>
+      <c r="Y21" t="n">
+        <v>4885</v>
+      </c>
+      <c r="Z21" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>5091</t>
         </is>
       </c>
     </row>
@@ -2236,7 +2366,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F22" s="5" t="n">
@@ -2296,9 +2426,15 @@
       <c r="X22" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>5575</t>
+      <c r="Y22" t="n">
+        <v>5575</v>
+      </c>
+      <c r="Z22" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>5890</t>
         </is>
       </c>
     </row>
@@ -2381,9 +2517,15 @@
       <c r="X23" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>5690</t>
+      <c r="Y23" t="n">
+        <v>5690</v>
+      </c>
+      <c r="Z23" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>6060</t>
         </is>
       </c>
     </row>
@@ -2466,9 +2608,15 @@
       <c r="X24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>5524</t>
+      <c r="Y24" t="n">
+        <v>5524</v>
+      </c>
+      <c r="Z24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>5613</t>
         </is>
       </c>
     </row>
@@ -2551,9 +2699,15 @@
       <c r="X25" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>5662</t>
+      <c r="Y25" t="n">
+        <v>5662</v>
+      </c>
+      <c r="Z25" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>5801</t>
         </is>
       </c>
     </row>
@@ -2636,9 +2790,15 @@
       <c r="X26" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>5610</t>
+      <c r="Y26" t="n">
+        <v>5610</v>
+      </c>
+      <c r="Z26" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>5864</t>
         </is>
       </c>
     </row>
@@ -2704,6 +2864,8 @@
       <c r="W27" t="inlineStr"/>
       <c r="X27" s="3" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
+      <c r="Z27" s="3" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2784,9 +2946,15 @@
       <c r="X28" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>6425</t>
+      <c r="Y28" t="n">
+        <v>6425</v>
+      </c>
+      <c r="Z28" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>6482</t>
         </is>
       </c>
     </row>
@@ -2869,9 +3037,15 @@
       <c r="X29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>5171</t>
+      <c r="Y29" t="n">
+        <v>5171</v>
+      </c>
+      <c r="Z29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>5597</t>
         </is>
       </c>
     </row>
@@ -2954,9 +3128,15 @@
       <c r="X30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>5519</t>
+      <c r="Y30" t="n">
+        <v>5519</v>
+      </c>
+      <c r="Z30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>5864</t>
         </is>
       </c>
     </row>
@@ -3039,9 +3219,15 @@
       <c r="X31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>5930</t>
+      <c r="Y31" t="n">
+        <v>5930</v>
+      </c>
+      <c r="Z31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>6234</t>
         </is>
       </c>
     </row>
@@ -3124,7 +3310,13 @@
       <c r="X32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y32" t="inlineStr">
+      <c r="Y32" t="n">
+        <v>4545</v>
+      </c>
+      <c r="Z32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="inlineStr">
         <is>
           <t>4545</t>
         </is>
@@ -3149,7 +3341,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F33" s="5" t="n">
@@ -3209,9 +3401,15 @@
       <c r="X33" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Y33" t="inlineStr">
-        <is>
-          <t>5944</t>
+      <c r="Y33" t="n">
+        <v>5944</v>
+      </c>
+      <c r="Z33" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>6010</t>
         </is>
       </c>
     </row>
@@ -3294,9 +3492,15 @@
       <c r="X34" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>5193</t>
+      <c r="Y34" t="n">
+        <v>5193</v>
+      </c>
+      <c r="Z34" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>5363</t>
         </is>
       </c>
     </row>
@@ -3379,9 +3583,15 @@
       <c r="X35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>4948</t>
+      <c r="Y35" t="n">
+        <v>4948</v>
+      </c>
+      <c r="Z35" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>5087</t>
         </is>
       </c>
     </row>
@@ -3404,7 +3614,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F36" s="3" t="n">
@@ -3464,9 +3674,15 @@
       <c r="X36" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>5521</t>
+      <c r="Y36" t="n">
+        <v>5521</v>
+      </c>
+      <c r="Z36" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>5743</t>
         </is>
       </c>
     </row>
@@ -3549,9 +3765,15 @@
       <c r="X37" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>5395</t>
+      <c r="Y37" t="n">
+        <v>5395</v>
+      </c>
+      <c r="Z37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>5627</t>
         </is>
       </c>
     </row>
@@ -3574,7 +3796,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F38" s="3" t="n">
@@ -3634,9 +3856,15 @@
       <c r="X38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>5466</t>
+      <c r="Y38" t="n">
+        <v>5466</v>
+      </c>
+      <c r="Z38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>5664</t>
         </is>
       </c>
     </row>
@@ -3719,9 +3947,15 @@
       <c r="X39" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>5527</t>
+      <c r="Y39" t="n">
+        <v>5527</v>
+      </c>
+      <c r="Z39" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>5905</t>
         </is>
       </c>
     </row>
@@ -3804,9 +4038,15 @@
       <c r="X40" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="Y40" t="inlineStr">
-        <is>
-          <t>6131</t>
+      <c r="Y40" t="n">
+        <v>6131</v>
+      </c>
+      <c r="Z40" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>6255</t>
         </is>
       </c>
     </row>
@@ -3829,7 +4069,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F41" s="5" t="n">
@@ -3889,9 +4129,15 @@
       <c r="X41" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>5703</t>
+      <c r="Y41" t="n">
+        <v>5703</v>
+      </c>
+      <c r="Z41" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>5839</t>
         </is>
       </c>
     </row>
@@ -3974,9 +4220,15 @@
       <c r="X42" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y42" t="inlineStr">
-        <is>
-          <t>4832</t>
+      <c r="Y42" t="n">
+        <v>4832</v>
+      </c>
+      <c r="Z42" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>4856</t>
         </is>
       </c>
     </row>
@@ -4059,9 +4311,15 @@
       <c r="X43" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="Y43" t="inlineStr">
-        <is>
-          <t>5721</t>
+      <c r="Y43" t="n">
+        <v>5721</v>
+      </c>
+      <c r="Z43" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA43" t="inlineStr">
+        <is>
+          <t>5803</t>
         </is>
       </c>
     </row>
@@ -4144,9 +4402,15 @@
       <c r="X44" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y44" t="inlineStr">
-        <is>
-          <t>5374</t>
+      <c r="Y44" t="n">
+        <v>5374</v>
+      </c>
+      <c r="Z44" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA44" t="inlineStr">
+        <is>
+          <t>5668</t>
         </is>
       </c>
     </row>
@@ -4229,9 +4493,15 @@
       <c r="X45" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Y45" t="inlineStr">
-        <is>
-          <t>5049</t>
+      <c r="Y45" t="n">
+        <v>5049</v>
+      </c>
+      <c r="Z45" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>5188</t>
         </is>
       </c>
     </row>
@@ -4254,7 +4524,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F46" s="5" t="n">
@@ -4314,9 +4584,15 @@
       <c r="X46" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>5213</t>
+      <c r="Y46" t="n">
+        <v>5213</v>
+      </c>
+      <c r="Z46" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>5452</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4615,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F47" s="5" t="n">
@@ -4399,9 +4675,15 @@
       <c r="X47" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="Y47" t="inlineStr">
-        <is>
-          <t>4725</t>
+      <c r="Y47" t="n">
+        <v>4725</v>
+      </c>
+      <c r="Z47" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>4988</t>
         </is>
       </c>
     </row>
@@ -4484,9 +4766,15 @@
       <c r="X48" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y48" t="inlineStr">
-        <is>
-          <t>5328</t>
+      <c r="Y48" t="n">
+        <v>5328</v>
+      </c>
+      <c r="Z48" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>5685</t>
         </is>
       </c>
     </row>
@@ -4569,9 +4857,15 @@
       <c r="X49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y49" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="Y49" t="n">
+        <v>4548</v>
+      </c>
+      <c r="Z49" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>5242</t>
         </is>
       </c>
     </row>
@@ -4654,9 +4948,15 @@
       <c r="X50" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y50" t="inlineStr">
-        <is>
-          <t>3145</t>
+      <c r="Y50" t="n">
+        <v>3145</v>
+      </c>
+      <c r="Z50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t>3169</t>
         </is>
       </c>
     </row>
@@ -4739,9 +5039,15 @@
       <c r="X51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y51" t="inlineStr">
-        <is>
-          <t>3304</t>
+      <c r="Y51" t="n">
+        <v>3304</v>
+      </c>
+      <c r="Z51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>3302</t>
         </is>
       </c>
     </row>
@@ -4824,9 +5130,15 @@
       <c r="X52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>4056</t>
+      <c r="Y52" t="n">
+        <v>4056</v>
+      </c>
+      <c r="Z52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>4456</t>
         </is>
       </c>
     </row>
@@ -4909,9 +5221,15 @@
       <c r="X53" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>4056</t>
+      <c r="Y53" t="n">
+        <v>4056</v>
+      </c>
+      <c r="Z53" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>4256</t>
         </is>
       </c>
     </row>
@@ -4994,9 +5312,15 @@
       <c r="X54" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>4373</t>
+      <c r="Y54" t="n">
+        <v>4373</v>
+      </c>
+      <c r="Z54" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>4474</t>
         </is>
       </c>
     </row>
@@ -5078,6 +5402,8 @@
       </c>
       <c r="X55" s="3" t="inlineStr"/>
       <c r="Y55" t="inlineStr"/>
+      <c r="Z55" s="3" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -5158,9 +5484,15 @@
       <c r="X56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>5073</t>
+      <c r="Y56" t="n">
+        <v>5073</v>
+      </c>
+      <c r="Z56" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>5210</t>
         </is>
       </c>
     </row>
@@ -5243,9 +5575,15 @@
       <c r="X57" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>4225</t>
+      <c r="Y57" t="n">
+        <v>4225</v>
+      </c>
+      <c r="Z57" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>4325</t>
         </is>
       </c>
     </row>
@@ -5328,9 +5666,15 @@
       <c r="X58" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>4977</t>
+      <c r="Y58" t="n">
+        <v>4977</v>
+      </c>
+      <c r="Z58" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>5158</t>
         </is>
       </c>
     </row>
@@ -5413,9 +5757,15 @@
       <c r="X59" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>5154</t>
+      <c r="Y59" t="n">
+        <v>5154</v>
+      </c>
+      <c r="Z59" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>5286</t>
         </is>
       </c>
     </row>
@@ -5498,9 +5848,15 @@
       <c r="X60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>4897</t>
+      <c r="Y60" t="n">
+        <v>4897</v>
+      </c>
+      <c r="Z60" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>5065</t>
         </is>
       </c>
     </row>
@@ -5583,9 +5939,15 @@
       <c r="X61" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>6604</t>
+      <c r="Y61" t="n">
+        <v>6604</v>
+      </c>
+      <c r="Z61" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>6889</t>
         </is>
       </c>
     </row>
@@ -5668,9 +6030,15 @@
       <c r="X62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>5008</t>
+      <c r="Y62" t="n">
+        <v>5008</v>
+      </c>
+      <c r="Z62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>5126</t>
         </is>
       </c>
     </row>
@@ -5753,9 +6121,15 @@
       <c r="X63" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>4333</t>
+      <c r="Y63" t="n">
+        <v>4333</v>
+      </c>
+      <c r="Z63" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>4477</t>
         </is>
       </c>
     </row>
@@ -5838,9 +6212,15 @@
       <c r="X64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>3857</t>
+      <c r="Y64" t="n">
+        <v>3857</v>
+      </c>
+      <c r="Z64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>4204</t>
         </is>
       </c>
     </row>
@@ -5923,9 +6303,15 @@
       <c r="X65" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="Y65" t="inlineStr">
-        <is>
-          <t>4320</t>
+      <c r="Y65" t="n">
+        <v>4320</v>
+      </c>
+      <c r="Z65" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA65" t="inlineStr">
+        <is>
+          <t>4497</t>
         </is>
       </c>
     </row>
@@ -6008,9 +6394,15 @@
       <c r="X66" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y66" t="inlineStr">
-        <is>
-          <t>5083</t>
+      <c r="Y66" t="n">
+        <v>5083</v>
+      </c>
+      <c r="Z66" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA66" t="inlineStr">
+        <is>
+          <t>5177</t>
         </is>
       </c>
     </row>
@@ -6093,9 +6485,15 @@
       <c r="X67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y67" t="inlineStr">
-        <is>
-          <t>4335</t>
+      <c r="Y67" t="n">
+        <v>4335</v>
+      </c>
+      <c r="Z67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA67" t="inlineStr">
+        <is>
+          <t>4478</t>
         </is>
       </c>
     </row>
@@ -6178,9 +6576,15 @@
       <c r="X68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y68" t="inlineStr">
-        <is>
-          <t>3536</t>
+      <c r="Y68" t="n">
+        <v>3536</v>
+      </c>
+      <c r="Z68" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>3860</t>
         </is>
       </c>
     </row>
@@ -6263,9 +6667,15 @@
       <c r="X69" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>3758</t>
+      <c r="Y69" t="n">
+        <v>3758</v>
+      </c>
+      <c r="Z69" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>3845</t>
         </is>
       </c>
     </row>
@@ -6348,9 +6758,15 @@
       <c r="X70" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y70" t="inlineStr">
-        <is>
-          <t>5409</t>
+      <c r="Y70" t="n">
+        <v>5409</v>
+      </c>
+      <c r="Z70" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>5637</t>
         </is>
       </c>
     </row>
@@ -6433,9 +6849,15 @@
       <c r="X71" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y71" t="inlineStr">
-        <is>
-          <t>5121</t>
+      <c r="Y71" t="n">
+        <v>5121</v>
+      </c>
+      <c r="Z71" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA71" t="inlineStr">
+        <is>
+          <t>5372</t>
         </is>
       </c>
     </row>
@@ -6518,9 +6940,15 @@
       <c r="X72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y72" t="inlineStr">
-        <is>
-          <t>4460</t>
+      <c r="Y72" t="n">
+        <v>4460</v>
+      </c>
+      <c r="Z72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>4544</t>
         </is>
       </c>
     </row>
@@ -6603,9 +7031,15 @@
       <c r="X73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y73" t="inlineStr">
-        <is>
-          <t>4922</t>
+      <c r="Y73" t="n">
+        <v>4922</v>
+      </c>
+      <c r="Z73" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>5068</t>
         </is>
       </c>
     </row>
@@ -6659,6 +7093,8 @@
       <c r="W74" t="inlineStr"/>
       <c r="X74" s="3" t="inlineStr"/>
       <c r="Y74" t="inlineStr"/>
+      <c r="Z74" s="3" t="inlineStr"/>
+      <c r="AA74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -6739,9 +7175,15 @@
       <c r="X75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Y75" t="inlineStr">
-        <is>
-          <t>4670</t>
+      <c r="Y75" t="n">
+        <v>4670</v>
+      </c>
+      <c r="Z75" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA75" t="inlineStr">
+        <is>
+          <t>4757</t>
         </is>
       </c>
     </row>
@@ -6824,9 +7266,15 @@
       <c r="X76" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="Y76" t="inlineStr">
-        <is>
-          <t>4604</t>
+      <c r="Y76" t="n">
+        <v>4604</v>
+      </c>
+      <c r="Z76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA76" t="inlineStr">
+        <is>
+          <t>4753</t>
         </is>
       </c>
     </row>
@@ -6909,9 +7357,15 @@
       <c r="X77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y77" t="inlineStr">
-        <is>
-          <t>4469</t>
+      <c r="Y77" t="n">
+        <v>4469</v>
+      </c>
+      <c r="Z77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>4492</t>
         </is>
       </c>
     </row>
@@ -6994,9 +7448,15 @@
       <c r="X78" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="Y78" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="Y78" t="n">
+        <v>3822</v>
+      </c>
+      <c r="Z78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA78" t="inlineStr">
+        <is>
+          <t>3874</t>
         </is>
       </c>
     </row>
@@ -7079,9 +7539,15 @@
       <c r="X79" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Y79" t="inlineStr">
-        <is>
-          <t>3552</t>
+      <c r="Y79" t="n">
+        <v>3552</v>
+      </c>
+      <c r="Z79" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA79" t="inlineStr">
+        <is>
+          <t>3643</t>
         </is>
       </c>
     </row>
@@ -7164,9 +7630,15 @@
       <c r="X80" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="Y80" t="inlineStr">
-        <is>
-          <t>4538</t>
+      <c r="Y80" t="n">
+        <v>4538</v>
+      </c>
+      <c r="Z80" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA80" t="inlineStr">
+        <is>
+          <t>4791</t>
         </is>
       </c>
     </row>
@@ -7249,9 +7721,15 @@
       <c r="X81" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Y81" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="Y81" t="n">
+        <v>2750</v>
+      </c>
+      <c r="Z81" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA81" t="inlineStr">
+        <is>
+          <t>2754</t>
         </is>
       </c>
     </row>
@@ -7334,9 +7812,15 @@
       <c r="X82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y82" t="inlineStr">
-        <is>
-          <t>3304</t>
+      <c r="Y82" t="n">
+        <v>3304</v>
+      </c>
+      <c r="Z82" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA82" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -7411,9 +7895,15 @@
       <c r="X83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y83" t="inlineStr">
-        <is>
-          <t>2319</t>
+      <c r="Y83" t="n">
+        <v>2319</v>
+      </c>
+      <c r="Z83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA83" t="inlineStr">
+        <is>
+          <t>2327</t>
         </is>
       </c>
     </row>
@@ -7496,9 +7986,15 @@
       <c r="X84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y84" t="inlineStr">
-        <is>
-          <t>2244</t>
+      <c r="Y84" t="n">
+        <v>2244</v>
+      </c>
+      <c r="Z84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA84" t="inlineStr">
+        <is>
+          <t>2259</t>
         </is>
       </c>
     </row>
@@ -7540,6 +8036,8 @@
       <c r="W85" t="inlineStr"/>
       <c r="X85" s="3" t="inlineStr"/>
       <c r="Y85" t="inlineStr"/>
+      <c r="Z85" s="3" t="inlineStr"/>
+      <c r="AA85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -7620,9 +8118,15 @@
       <c r="X86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y86" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="Y86" t="n">
+        <v>2534</v>
+      </c>
+      <c r="Z86" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA86" t="inlineStr">
+        <is>
+          <t>2586</t>
         </is>
       </c>
     </row>
@@ -7705,9 +8209,15 @@
       <c r="X87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y87" t="inlineStr">
-        <is>
-          <t>3211</t>
+      <c r="Y87" t="n">
+        <v>3211</v>
+      </c>
+      <c r="Z87" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA87" t="inlineStr">
+        <is>
+          <t>3337</t>
         </is>
       </c>
     </row>
@@ -7761,6 +8271,8 @@
       <c r="W88" t="inlineStr"/>
       <c r="X88" s="3" t="inlineStr"/>
       <c r="Y88" t="inlineStr"/>
+      <c r="Z88" s="3" t="inlineStr"/>
+      <c r="AA88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -7841,9 +8353,15 @@
       <c r="X89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y89" t="inlineStr">
-        <is>
-          <t>2337</t>
+      <c r="Y89" t="n">
+        <v>2337</v>
+      </c>
+      <c r="Z89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA89" t="inlineStr">
+        <is>
+          <t>2342</t>
         </is>
       </c>
     </row>
@@ -7926,9 +8444,15 @@
       <c r="X90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y90" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="Y90" t="n">
+        <v>2903</v>
+      </c>
+      <c r="Z90" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA90" t="inlineStr">
+        <is>
+          <t>3005</t>
         </is>
       </c>
     </row>
@@ -8011,9 +8535,15 @@
       <c r="X91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y91" t="inlineStr">
-        <is>
-          <t>3354</t>
+      <c r="Y91" t="n">
+        <v>3354</v>
+      </c>
+      <c r="Z91" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA91" t="inlineStr">
+        <is>
+          <t>3480</t>
         </is>
       </c>
     </row>
@@ -8096,9 +8626,15 @@
       <c r="X92" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Y92" t="inlineStr">
-        <is>
-          <t>3361</t>
+      <c r="Y92" t="n">
+        <v>3361</v>
+      </c>
+      <c r="Z92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -8181,9 +8717,15 @@
       <c r="X93" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y93" t="inlineStr">
-        <is>
-          <t>4307</t>
+      <c r="Y93" t="n">
+        <v>4307</v>
+      </c>
+      <c r="Z93" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA93" t="inlineStr">
+        <is>
+          <t>4420</t>
         </is>
       </c>
     </row>
@@ -8266,9 +8808,15 @@
       <c r="X94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y94" t="inlineStr">
-        <is>
-          <t>4001</t>
+      <c r="Y94" t="n">
+        <v>4001</v>
+      </c>
+      <c r="Z94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA94" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -8351,9 +8899,15 @@
       <c r="X95" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y95" t="inlineStr">
-        <is>
-          <t>3950</t>
+      <c r="Y95" t="n">
+        <v>3950</v>
+      </c>
+      <c r="Z95" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA95" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -8436,9 +8990,15 @@
       <c r="X96" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="Y96" t="inlineStr">
-        <is>
-          <t>4513</t>
+      <c r="Y96" t="n">
+        <v>4513</v>
+      </c>
+      <c r="Z96" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA96" t="inlineStr">
+        <is>
+          <t>4658</t>
         </is>
       </c>
     </row>
@@ -8492,6 +9052,8 @@
       <c r="W97" t="inlineStr"/>
       <c r="X97" s="3" t="inlineStr"/>
       <c r="Y97" t="inlineStr"/>
+      <c r="Z97" s="3" t="inlineStr"/>
+      <c r="AA97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -8572,9 +9134,15 @@
       <c r="X98" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y98" t="inlineStr">
-        <is>
-          <t>2964</t>
+      <c r="Y98" t="n">
+        <v>2964</v>
+      </c>
+      <c r="Z98" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA98" t="inlineStr">
+        <is>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -8657,9 +9225,15 @@
       <c r="X99" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Y99" t="inlineStr">
-        <is>
-          <t>3973</t>
+      <c r="Y99" t="n">
+        <v>3973</v>
+      </c>
+      <c r="Z99" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA99" t="inlineStr">
+        <is>
+          <t>4045</t>
         </is>
       </c>
     </row>
@@ -8742,9 +9316,15 @@
       <c r="X100" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y100" t="inlineStr">
-        <is>
-          <t>3545</t>
+      <c r="Y100" t="n">
+        <v>3545</v>
+      </c>
+      <c r="Z100" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA100" t="inlineStr">
+        <is>
+          <t>3642</t>
         </is>
       </c>
     </row>
@@ -8827,9 +9407,15 @@
       <c r="X101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y101" t="inlineStr">
-        <is>
-          <t>2637</t>
+      <c r="Y101" t="n">
+        <v>2637</v>
+      </c>
+      <c r="Z101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA101" t="inlineStr">
+        <is>
+          <t>2678</t>
         </is>
       </c>
     </row>
@@ -8912,9 +9498,15 @@
       <c r="X102" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="Y102" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="Y102" t="n">
+        <v>2712</v>
+      </c>
+      <c r="Z102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA102" t="inlineStr">
+        <is>
+          <t>2727</t>
         </is>
       </c>
     </row>
@@ -8997,9 +9589,15 @@
       <c r="X103" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y103" t="inlineStr">
-        <is>
-          <t>3397</t>
+      <c r="Y103" t="n">
+        <v>3397</v>
+      </c>
+      <c r="Z103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA103" t="inlineStr">
+        <is>
+          <t>3404</t>
         </is>
       </c>
     </row>
@@ -9082,9 +9680,15 @@
       <c r="X104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y104" t="inlineStr">
-        <is>
-          <t>3735</t>
+      <c r="Y104" t="n">
+        <v>3735</v>
+      </c>
+      <c r="Z104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA104" t="inlineStr">
+        <is>
+          <t>3808</t>
         </is>
       </c>
     </row>
@@ -9138,6 +9742,8 @@
       <c r="W105" t="inlineStr"/>
       <c r="X105" s="3" t="inlineStr"/>
       <c r="Y105" t="inlineStr"/>
+      <c r="Z105" s="3" t="inlineStr"/>
+      <c r="AA105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9177,6 +9783,8 @@
       <c r="W106" t="inlineStr"/>
       <c r="X106" s="3" t="inlineStr"/>
       <c r="Y106" t="inlineStr"/>
+      <c r="Z106" s="3" t="inlineStr"/>
+      <c r="AA106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9244,6 +9852,8 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" s="3" t="inlineStr"/>
       <c r="Y107" t="inlineStr"/>
+      <c r="Z107" s="3" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9324,9 +9934,15 @@
       <c r="X108" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Y108" t="inlineStr">
-        <is>
-          <t>2775</t>
+      <c r="Y108" t="n">
+        <v>2775</v>
+      </c>
+      <c r="Z108" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA108" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -9409,9 +10025,15 @@
       <c r="X109" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y109" t="inlineStr">
-        <is>
-          <t>3460</t>
+      <c r="Y109" t="n">
+        <v>3460</v>
+      </c>
+      <c r="Z109" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA109" t="inlineStr">
+        <is>
+          <t>3589</t>
         </is>
       </c>
     </row>
@@ -9494,9 +10116,15 @@
       <c r="X110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y110" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="Y110" t="n">
+        <v>3339</v>
+      </c>
+      <c r="Z110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA110" t="inlineStr">
+        <is>
+          <t>3469</t>
         </is>
       </c>
     </row>
@@ -9579,9 +10207,15 @@
       <c r="X111" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y111" t="inlineStr">
-        <is>
-          <t>4433</t>
+      <c r="Y111" t="n">
+        <v>4433</v>
+      </c>
+      <c r="Z111" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA111" t="inlineStr">
+        <is>
+          <t>4451</t>
         </is>
       </c>
     </row>
@@ -9664,9 +10298,15 @@
       <c r="X112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y112" t="inlineStr">
-        <is>
-          <t>3455</t>
+      <c r="Y112" t="n">
+        <v>3455</v>
+      </c>
+      <c r="Z112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA112" t="inlineStr">
+        <is>
+          <t>3499</t>
         </is>
       </c>
     </row>
@@ -9749,9 +10389,15 @@
       <c r="X113" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>4381</t>
+      <c r="Y113" t="n">
+        <v>4381</v>
+      </c>
+      <c r="Z113" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA113" t="inlineStr">
+        <is>
+          <t>4585</t>
         </is>
       </c>
     </row>
@@ -9834,9 +10480,15 @@
       <c r="X114" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y114" t="inlineStr">
-        <is>
-          <t>3180</t>
+      <c r="Y114" t="n">
+        <v>3180</v>
+      </c>
+      <c r="Z114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA114" t="inlineStr">
+        <is>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -9919,9 +10571,15 @@
       <c r="X115" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Y115" t="inlineStr">
-        <is>
-          <t>3672</t>
+      <c r="Y115" t="n">
+        <v>3672</v>
+      </c>
+      <c r="Z115" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>3706</t>
         </is>
       </c>
     </row>
@@ -10004,9 +10662,15 @@
       <c r="X116" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="Y116" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="Y116" t="n">
+        <v>2998</v>
+      </c>
+      <c r="Z116" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA116" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -10089,9 +10753,15 @@
       <c r="X117" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y117" t="inlineStr">
-        <is>
-          <t>3033</t>
+      <c r="Y117" t="n">
+        <v>3033</v>
+      </c>
+      <c r="Z117" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA117" t="inlineStr">
+        <is>
+          <t>3091</t>
         </is>
       </c>
     </row>
@@ -10174,9 +10844,15 @@
       <c r="X118" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y118" t="inlineStr">
-        <is>
-          <t>3202</t>
+      <c r="Y118" t="n">
+        <v>3202</v>
+      </c>
+      <c r="Z118" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA118" t="inlineStr">
+        <is>
+          <t>3350</t>
         </is>
       </c>
     </row>
@@ -10259,9 +10935,15 @@
       <c r="X119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y119" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="Y119" t="n">
+        <v>3182</v>
+      </c>
+      <c r="Z119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA119" t="inlineStr">
+        <is>
+          <t>3200</t>
         </is>
       </c>
     </row>
@@ -10344,9 +11026,15 @@
       <c r="X120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y120" t="inlineStr">
-        <is>
-          <t>3393</t>
+      <c r="Y120" t="n">
+        <v>3393</v>
+      </c>
+      <c r="Z120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA120" t="inlineStr">
+        <is>
+          <t>3456</t>
         </is>
       </c>
     </row>
@@ -10409,9 +11097,15 @@
       <c r="X121" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y121" t="inlineStr">
-        <is>
-          <t>3209</t>
+      <c r="Y121" t="n">
+        <v>3209</v>
+      </c>
+      <c r="Z121" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA121" t="inlineStr">
+        <is>
+          <t>3297</t>
         </is>
       </c>
     </row>
@@ -10494,9 +11188,15 @@
       <c r="X122" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Y122" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="Y122" t="n">
+        <v>2519</v>
+      </c>
+      <c r="Z122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA122" t="inlineStr">
+        <is>
+          <t>2488</t>
         </is>
       </c>
     </row>
@@ -10550,6 +11250,8 @@
       <c r="W123" t="inlineStr"/>
       <c r="X123" s="3" t="inlineStr"/>
       <c r="Y123" t="inlineStr"/>
+      <c r="Z123" s="3" t="inlineStr"/>
+      <c r="AA123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -10601,6 +11303,8 @@
       <c r="W124" t="inlineStr"/>
       <c r="X124" s="3" t="inlineStr"/>
       <c r="Y124" t="inlineStr"/>
+      <c r="Z124" s="3" t="inlineStr"/>
+      <c r="AA124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -10681,9 +11385,15 @@
       <c r="X125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y125" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="Y125" t="n">
+        <v>2605</v>
+      </c>
+      <c r="Z125" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA125" t="inlineStr">
+        <is>
+          <t>2593</t>
         </is>
       </c>
     </row>
@@ -10733,6 +11443,8 @@
       <c r="W126" t="inlineStr"/>
       <c r="X126" s="3" t="inlineStr"/>
       <c r="Y126" t="inlineStr"/>
+      <c r="Z126" s="3" t="inlineStr"/>
+      <c r="AA126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -10813,9 +11525,15 @@
       <c r="X127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y127" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="Y127" t="n">
+        <v>2809</v>
+      </c>
+      <c r="Z127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA127" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -10898,9 +11616,15 @@
       <c r="X128" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y128" t="inlineStr">
-        <is>
-          <t>3698</t>
+      <c r="Y128" t="n">
+        <v>3698</v>
+      </c>
+      <c r="Z128" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA128" t="inlineStr">
+        <is>
+          <t>3804</t>
         </is>
       </c>
     </row>
@@ -10950,6 +11674,8 @@
       <c r="W129" t="inlineStr"/>
       <c r="X129" s="3" t="inlineStr"/>
       <c r="Y129" t="inlineStr"/>
+      <c r="Z129" s="3" t="inlineStr"/>
+      <c r="AA129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -11030,7 +11756,13 @@
       <c r="X130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y130" t="inlineStr">
+      <c r="Y130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11082,6 +11814,8 @@
       <c r="W131" t="inlineStr"/>
       <c r="X131" s="3" t="inlineStr"/>
       <c r="Y131" t="inlineStr"/>
+      <c r="Z131" s="3" t="inlineStr"/>
+      <c r="AA131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -11162,9 +11896,15 @@
       <c r="X132" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="Y132" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="Y132" t="n">
+        <v>2719</v>
+      </c>
+      <c r="Z132" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA132" t="inlineStr">
+        <is>
+          <t>2754</t>
         </is>
       </c>
     </row>
@@ -11247,9 +11987,15 @@
       <c r="X133" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y133" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="Y133" t="n">
+        <v>2885</v>
+      </c>
+      <c r="Z133" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA133" t="inlineStr">
+        <is>
+          <t>2879</t>
         </is>
       </c>
     </row>
@@ -11299,6 +12045,8 @@
       <c r="W134" t="inlineStr"/>
       <c r="X134" s="3" t="inlineStr"/>
       <c r="Y134" t="inlineStr"/>
+      <c r="Z134" s="3" t="inlineStr"/>
+      <c r="AA134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -11346,6 +12094,8 @@
       <c r="W135" t="inlineStr"/>
       <c r="X135" s="3" t="inlineStr"/>
       <c r="Y135" t="inlineStr"/>
+      <c r="Z135" s="3" t="inlineStr"/>
+      <c r="AA135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -11426,9 +12176,15 @@
       <c r="X136" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="Y136" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="Y136" t="n">
+        <v>2552</v>
+      </c>
+      <c r="Z136" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA136" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -11478,6 +12234,8 @@
       <c r="W137" t="inlineStr"/>
       <c r="X137" s="3" t="inlineStr"/>
       <c r="Y137" t="inlineStr"/>
+      <c r="Z137" s="3" t="inlineStr"/>
+      <c r="AA137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -11525,6 +12283,8 @@
       <c r="W138" t="inlineStr"/>
       <c r="X138" s="3" t="inlineStr"/>
       <c r="Y138" t="inlineStr"/>
+      <c r="Z138" s="3" t="inlineStr"/>
+      <c r="AA138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -11605,9 +12365,15 @@
       <c r="X139" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Y139" t="inlineStr">
-        <is>
-          <t>2376</t>
+      <c r="Y139" t="n">
+        <v>2376</v>
+      </c>
+      <c r="Z139" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA139" t="inlineStr">
+        <is>
+          <t>2404</t>
         </is>
       </c>
     </row>
@@ -11690,9 +12456,15 @@
       <c r="X140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y140" t="inlineStr">
-        <is>
-          <t>1823</t>
+      <c r="Y140" t="n">
+        <v>1823</v>
+      </c>
+      <c r="Z140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA140" t="inlineStr">
+        <is>
+          <t>1816</t>
         </is>
       </c>
     </row>
@@ -11742,6 +12514,8 @@
       <c r="W141" t="inlineStr"/>
       <c r="X141" s="3" t="inlineStr"/>
       <c r="Y141" t="inlineStr"/>
+      <c r="Z141" s="3" t="inlineStr"/>
+      <c r="AA141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -11822,7 +12596,13 @@
       <c r="X142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y142" t="inlineStr">
+      <c r="Y142" t="n">
+        <v>2160</v>
+      </c>
+      <c r="Z142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA142" t="inlineStr">
         <is>
           <t>2160</t>
         </is>
@@ -11907,9 +12687,15 @@
       <c r="X143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y143" t="inlineStr">
-        <is>
-          <t>1535</t>
+      <c r="Y143" t="n">
+        <v>1535</v>
+      </c>
+      <c r="Z143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA143" t="inlineStr">
+        <is>
+          <t>1533</t>
         </is>
       </c>
     </row>
@@ -11968,7 +12754,13 @@
       <c r="X144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y144" t="inlineStr">
+      <c r="Y144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12020,6 +12812,8 @@
       <c r="W145" t="inlineStr"/>
       <c r="X145" s="3" t="inlineStr"/>
       <c r="Y145" t="inlineStr"/>
+      <c r="Z145" s="3" t="inlineStr"/>
+      <c r="AA145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -12100,9 +12894,15 @@
       <c r="X146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y146" t="inlineStr">
-        <is>
-          <t>2403</t>
+      <c r="Y146" t="n">
+        <v>2403</v>
+      </c>
+      <c r="Z146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA146" t="inlineStr">
+        <is>
+          <t>2418</t>
         </is>
       </c>
     </row>
@@ -12185,7 +12985,13 @@
       <c r="X147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y147" t="inlineStr">
+      <c r="Y147" t="n">
+        <v>2256</v>
+      </c>
+      <c r="Z147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA147" t="inlineStr">
         <is>
           <t>2256</t>
         </is>
@@ -12237,6 +13043,8 @@
       <c r="W148" t="inlineStr"/>
       <c r="X148" s="3" t="inlineStr"/>
       <c r="Y148" t="inlineStr"/>
+      <c r="Z148" s="3" t="inlineStr"/>
+      <c r="AA148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -12284,6 +13092,8 @@
       <c r="W149" t="inlineStr"/>
       <c r="X149" s="3" t="inlineStr"/>
       <c r="Y149" t="inlineStr"/>
+      <c r="Z149" s="3" t="inlineStr"/>
+      <c r="AA149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -12331,6 +13141,8 @@
       <c r="W150" t="inlineStr"/>
       <c r="X150" s="3" t="inlineStr"/>
       <c r="Y150" t="inlineStr"/>
+      <c r="Z150" s="3" t="inlineStr"/>
+      <c r="AA150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -12411,9 +13223,15 @@
       <c r="X151" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="Y151" t="inlineStr">
-        <is>
-          <t>4796</t>
+      <c r="Y151" t="n">
+        <v>4796</v>
+      </c>
+      <c r="Z151" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA151" t="inlineStr">
+        <is>
+          <t>4949</t>
         </is>
       </c>
     </row>
@@ -12496,7 +13314,13 @@
       <c r="X152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y152" t="inlineStr">
+      <c r="Y152" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12581,9 +13405,15 @@
       <c r="X153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y153" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="Y153" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Z153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA153" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -12666,9 +13496,15 @@
       <c r="X154" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Y154" t="inlineStr">
-        <is>
-          <t>3782</t>
+      <c r="Y154" t="n">
+        <v>3782</v>
+      </c>
+      <c r="Z154" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA154" t="inlineStr">
+        <is>
+          <t>4286</t>
         </is>
       </c>
     </row>
@@ -12751,7 +13587,13 @@
       <c r="X155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y155" t="inlineStr">
+      <c r="Y155" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12836,9 +13678,15 @@
       <c r="X156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y156" t="inlineStr">
-        <is>
-          <t>2777</t>
+      <c r="Y156" t="n">
+        <v>2777</v>
+      </c>
+      <c r="Z156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA156" t="inlineStr">
+        <is>
+          <t>2788</t>
         </is>
       </c>
     </row>
@@ -12904,6 +13752,8 @@
       <c r="W157" t="inlineStr"/>
       <c r="X157" s="3" t="inlineStr"/>
       <c r="Y157" t="inlineStr"/>
+      <c r="Z157" s="3" t="inlineStr"/>
+      <c r="AA157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -12984,7 +13834,13 @@
       <c r="X158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y158" t="inlineStr">
+      <c r="Y158" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13069,9 +13925,15 @@
       <c r="X159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y159" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="Y159" t="n">
+        <v>3236</v>
+      </c>
+      <c r="Z159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA159" t="inlineStr">
+        <is>
+          <t>3235</t>
         </is>
       </c>
     </row>
@@ -13088,7 +13950,7 @@
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F160" s="5" t="n">
@@ -13148,9 +14010,15 @@
       <c r="X160" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y160" t="inlineStr">
-        <is>
-          <t>5721</t>
+      <c r="Y160" t="n">
+        <v>5721</v>
+      </c>
+      <c r="Z160" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA160" t="inlineStr">
+        <is>
+          <t>6129</t>
         </is>
       </c>
     </row>
@@ -13227,9 +14095,15 @@
       <c r="X161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y161" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="Y161" t="n">
+        <v>2551</v>
+      </c>
+      <c r="Z161" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA161" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
@@ -13273,6 +14147,8 @@
       <c r="W162" t="inlineStr"/>
       <c r="X162" s="3" t="inlineStr"/>
       <c r="Y162" t="inlineStr"/>
+      <c r="Z162" s="3" t="inlineStr"/>
+      <c r="AA162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -13326,6 +14202,8 @@
       <c r="W163" t="inlineStr"/>
       <c r="X163" s="3" t="inlineStr"/>
       <c r="Y163" t="inlineStr"/>
+      <c r="Z163" s="3" t="inlineStr"/>
+      <c r="AA163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -13384,9 +14262,15 @@
       <c r="X164" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y164" t="inlineStr">
-        <is>
-          <t>4595</t>
+      <c r="Y164" t="n">
+        <v>4595</v>
+      </c>
+      <c r="Z164" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA164" t="inlineStr">
+        <is>
+          <t>4707</t>
         </is>
       </c>
     </row>
@@ -13447,9 +14331,15 @@
       <c r="X165" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y165" t="inlineStr">
-        <is>
-          <t>3815</t>
+      <c r="Y165" t="n">
+        <v>3815</v>
+      </c>
+      <c r="Z165" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA165" t="inlineStr">
+        <is>
+          <t>4071</t>
         </is>
       </c>
     </row>
@@ -13506,9 +14396,15 @@
       <c r="X166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y166" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="Y166" t="n">
+        <v>2554</v>
+      </c>
+      <c r="Z166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA166" t="inlineStr">
+        <is>
+          <t>2569</t>
         </is>
       </c>
     </row>
@@ -13552,6 +14448,8 @@
       <c r="W167" t="inlineStr"/>
       <c r="X167" s="3" t="inlineStr"/>
       <c r="Y167" t="inlineStr"/>
+      <c r="Z167" s="3" t="inlineStr"/>
+      <c r="AA167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -13606,9 +14504,15 @@
       <c r="X168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y168" t="inlineStr">
-        <is>
-          <t>1659</t>
+      <c r="Y168" t="n">
+        <v>1659</v>
+      </c>
+      <c r="Z168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA168" t="inlineStr">
+        <is>
+          <t>1645</t>
         </is>
       </c>
     </row>
@@ -13661,9 +14565,15 @@
       <c r="X169" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y169" t="inlineStr">
-        <is>
-          <t>4076</t>
+      <c r="Y169" t="n">
+        <v>4076</v>
+      </c>
+      <c r="Z169" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA169" t="inlineStr">
+        <is>
+          <t>4071</t>
         </is>
       </c>
     </row>
@@ -13712,9 +14622,15 @@
       <c r="X170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y170" t="inlineStr">
-        <is>
-          <t>2081</t>
+      <c r="Y170" t="n">
+        <v>2081</v>
+      </c>
+      <c r="Z170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA170" t="inlineStr">
+        <is>
+          <t>2067</t>
         </is>
       </c>
     </row>
@@ -13758,6 +14674,8 @@
       <c r="W171" t="inlineStr"/>
       <c r="X171" s="3" t="inlineStr"/>
       <c r="Y171" t="inlineStr"/>
+      <c r="Z171" s="3" t="inlineStr"/>
+      <c r="AA171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -13800,9 +14718,15 @@
       <c r="X172" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y172" t="inlineStr">
-        <is>
-          <t>3244</t>
+      <c r="Y172" t="n">
+        <v>3244</v>
+      </c>
+      <c r="Z172" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA172" t="inlineStr">
+        <is>
+          <t>3270</t>
         </is>
       </c>
     </row>
@@ -13846,12 +14770,12 @@
       </c>
       <c r="X173" s="3" t="inlineStr"/>
       <c r="Y173" t="inlineStr"/>
+      <c r="Z173" s="3" t="inlineStr"/>
+      <c r="AA173" t="inlineStr"/>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>58382408</t>
-        </is>
+      <c r="A174" t="n">
+        <v>58382408</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -13886,9 +14810,62 @@
       <c r="X174" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Y174" t="inlineStr">
-        <is>
-          <t>1097</t>
+      <c r="Y174" t="n">
+        <v>1097</v>
+      </c>
+      <c r="Z174" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA174" t="inlineStr">
+        <is>
+          <t>1092</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>58310362</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>不老实的老实人</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F175" s="3" t="inlineStr"/>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" s="3" t="inlineStr"/>
+      <c r="I175" t="inlineStr"/>
+      <c r="J175" s="3" t="inlineStr"/>
+      <c r="K175" t="inlineStr"/>
+      <c r="L175" s="3" t="inlineStr"/>
+      <c r="M175" t="inlineStr"/>
+      <c r="N175" s="3" t="inlineStr"/>
+      <c r="O175" t="inlineStr"/>
+      <c r="P175" s="3" t="inlineStr"/>
+      <c r="Q175" t="inlineStr"/>
+      <c r="R175" s="3" t="inlineStr"/>
+      <c r="S175" t="inlineStr"/>
+      <c r="T175" s="3" t="inlineStr"/>
+      <c r="U175" t="inlineStr"/>
+      <c r="V175" s="3" t="inlineStr"/>
+      <c r="W175" t="inlineStr"/>
+      <c r="X175" s="3" t="inlineStr"/>
+      <c r="Y175" t="inlineStr"/>
+      <c r="Z175" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA175" t="inlineStr">
+        <is>
+          <t>1627</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 22-12-30 14:54:08
</commit_message>
<xml_diff>
--- a/Season_Attack/80.xlsx
+++ b/Season_Attack/80.xlsx
@@ -14823,10 +14823,8 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>58310362</t>
-        </is>
+      <c r="A175" t="n">
+        <v>58310362</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-01-03 09:53:25
</commit_message>
<xml_diff>
--- a/Season_Attack/80.xlsx
+++ b/Season_Attack/80.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA175"/>
+  <dimension ref="A1:AC177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,16 @@
           <t>12-29_0</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>12-31_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>12-31_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -612,9 +622,15 @@
       <c r="Z2" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>3895</t>
+      <c r="AA2" t="n">
+        <v>3895</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>4280</t>
         </is>
       </c>
     </row>
@@ -703,9 +719,15 @@
       <c r="Z3" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>5259</t>
+      <c r="AA3" t="n">
+        <v>5259</v>
+      </c>
+      <c r="AB3" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>6013</t>
         </is>
       </c>
     </row>
@@ -794,9 +816,15 @@
       <c r="Z4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>4491</t>
+      <c r="AA4" t="n">
+        <v>4491</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -885,9 +913,15 @@
       <c r="Z5" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>6125</t>
+      <c r="AA5" t="n">
+        <v>6125</v>
+      </c>
+      <c r="AB5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>6453</t>
         </is>
       </c>
     </row>
@@ -910,7 +944,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
@@ -976,9 +1010,15 @@
       <c r="Z6" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>6192</t>
+      <c r="AA6" t="n">
+        <v>6192</v>
+      </c>
+      <c r="AB6" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>6537</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1041,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F7" s="5" t="n">
@@ -1067,9 +1107,15 @@
       <c r="Z7" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>6234</t>
+      <c r="AA7" t="n">
+        <v>6234</v>
+      </c>
+      <c r="AB7" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>6661</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1138,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F8" s="3" t="n">
@@ -1158,9 +1204,15 @@
       <c r="Z8" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>5436</t>
+      <c r="AA8" t="n">
+        <v>5436</v>
+      </c>
+      <c r="AB8" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>5816</t>
         </is>
       </c>
     </row>
@@ -1249,9 +1301,15 @@
       <c r="Z9" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>5598</t>
+      <c r="AA9" t="n">
+        <v>5598</v>
+      </c>
+      <c r="AB9" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>5835</t>
         </is>
       </c>
     </row>
@@ -1340,9 +1398,15 @@
       <c r="Z10" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>5720</t>
+      <c r="AA10" t="n">
+        <v>5720</v>
+      </c>
+      <c r="AB10" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>6084</t>
         </is>
       </c>
     </row>
@@ -1431,9 +1495,15 @@
       <c r="Z11" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>6739</t>
+      <c r="AA11" t="n">
+        <v>6739</v>
+      </c>
+      <c r="AB11" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>7163</t>
         </is>
       </c>
     </row>
@@ -1522,9 +1592,15 @@
       <c r="Z12" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA12" t="inlineStr">
-        <is>
-          <t>5463</t>
+      <c r="AA12" t="n">
+        <v>5463</v>
+      </c>
+      <c r="AB12" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>5878</t>
         </is>
       </c>
     </row>
@@ -1613,9 +1689,15 @@
       <c r="Z13" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>5341</t>
+      <c r="AA13" t="n">
+        <v>5341</v>
+      </c>
+      <c r="AB13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>5623</t>
         </is>
       </c>
     </row>
@@ -1704,9 +1786,15 @@
       <c r="Z14" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>6327</t>
+      <c r="AA14" t="n">
+        <v>6327</v>
+      </c>
+      <c r="AB14" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>6485</t>
         </is>
       </c>
     </row>
@@ -1795,9 +1883,15 @@
       <c r="Z15" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA15" t="inlineStr">
-        <is>
-          <t>5432</t>
+      <c r="AA15" t="n">
+        <v>5432</v>
+      </c>
+      <c r="AB15" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>5682</t>
         </is>
       </c>
     </row>
@@ -1886,9 +1980,15 @@
       <c r="Z16" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>6306</t>
+      <c r="AA16" t="n">
+        <v>6306</v>
+      </c>
+      <c r="AB16" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>7037</t>
         </is>
       </c>
     </row>
@@ -1977,9 +2077,15 @@
       <c r="Z17" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>5609</t>
+      <c r="AA17" t="n">
+        <v>5609</v>
+      </c>
+      <c r="AB17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>5948</t>
         </is>
       </c>
     </row>
@@ -2002,7 +2108,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F18" s="3" t="n">
@@ -2068,9 +2174,15 @@
       <c r="Z18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>5159</t>
+      <c r="AA18" t="n">
+        <v>5159</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>5607</t>
         </is>
       </c>
     </row>
@@ -2159,9 +2271,15 @@
       <c r="Z19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>5957</t>
+      <c r="AA19" t="n">
+        <v>5957</v>
+      </c>
+      <c r="AB19" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>6434</t>
         </is>
       </c>
     </row>
@@ -2184,7 +2302,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F20" s="5" t="n">
@@ -2250,9 +2368,15 @@
       <c r="Z20" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>5805</t>
+      <c r="AA20" t="n">
+        <v>5805</v>
+      </c>
+      <c r="AB20" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>6622</t>
         </is>
       </c>
     </row>
@@ -2341,9 +2465,15 @@
       <c r="Z21" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>5091</t>
+      <c r="AA21" t="n">
+        <v>5091</v>
+      </c>
+      <c r="AB21" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>5627</t>
         </is>
       </c>
     </row>
@@ -2432,9 +2562,15 @@
       <c r="Z22" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>5890</t>
+      <c r="AA22" t="n">
+        <v>5890</v>
+      </c>
+      <c r="AB22" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>6392</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2593,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F23" s="2" t="n">
@@ -2523,9 +2659,15 @@
       <c r="Z23" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>6060</t>
+      <c r="AA23" t="n">
+        <v>6060</v>
+      </c>
+      <c r="AB23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>6179</t>
         </is>
       </c>
     </row>
@@ -2548,7 +2690,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F24" s="5" t="n">
@@ -2614,9 +2756,15 @@
       <c r="Z24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>5613</t>
+      <c r="AA24" t="n">
+        <v>5613</v>
+      </c>
+      <c r="AB24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>5932</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2787,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F25" s="5" t="n">
@@ -2705,9 +2853,15 @@
       <c r="Z25" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>5801</t>
+      <c r="AA25" t="n">
+        <v>5801</v>
+      </c>
+      <c r="AB25" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>5944</t>
         </is>
       </c>
     </row>
@@ -2796,9 +2950,15 @@
       <c r="Z26" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>5864</t>
+      <c r="AA26" t="n">
+        <v>5864</v>
+      </c>
+      <c r="AB26" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>6259</t>
         </is>
       </c>
     </row>
@@ -2866,6 +3026,8 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" s="3" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
+      <c r="AB27" s="3" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2886,7 +3048,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F28" s="2" t="n">
@@ -2952,9 +3114,15 @@
       <c r="Z28" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AA28" t="inlineStr">
-        <is>
-          <t>6482</t>
+      <c r="AA28" t="n">
+        <v>6482</v>
+      </c>
+      <c r="AB28" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>6629</t>
         </is>
       </c>
     </row>
@@ -2977,7 +3145,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F29" s="3" t="n">
@@ -3043,9 +3211,15 @@
       <c r="Z29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>5597</t>
+      <c r="AA29" t="n">
+        <v>5597</v>
+      </c>
+      <c r="AB29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>6388</t>
         </is>
       </c>
     </row>
@@ -3134,9 +3308,15 @@
       <c r="Z30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>5864</t>
+      <c r="AA30" t="n">
+        <v>5864</v>
+      </c>
+      <c r="AB30" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>6264</t>
         </is>
       </c>
     </row>
@@ -3159,7 +3339,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F31" s="5" t="n">
@@ -3225,9 +3405,15 @@
       <c r="Z31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>6234</t>
+      <c r="AA31" t="n">
+        <v>6234</v>
+      </c>
+      <c r="AB31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>6805</t>
         </is>
       </c>
     </row>
@@ -3316,9 +3502,15 @@
       <c r="Z32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>4545</t>
+      <c r="AA32" t="n">
+        <v>4545</v>
+      </c>
+      <c r="AB32" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>4574</t>
         </is>
       </c>
     </row>
@@ -3407,9 +3599,15 @@
       <c r="Z33" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA33" t="inlineStr">
-        <is>
-          <t>6010</t>
+      <c r="AA33" t="n">
+        <v>6010</v>
+      </c>
+      <c r="AB33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>6424</t>
         </is>
       </c>
     </row>
@@ -3498,9 +3696,15 @@
       <c r="Z34" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>5363</t>
+      <c r="AA34" t="n">
+        <v>5363</v>
+      </c>
+      <c r="AB34" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>5838</t>
         </is>
       </c>
     </row>
@@ -3589,9 +3793,15 @@
       <c r="Z35" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>5087</t>
+      <c r="AA35" t="n">
+        <v>5087</v>
+      </c>
+      <c r="AB35" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>5251</t>
         </is>
       </c>
     </row>
@@ -3680,9 +3890,15 @@
       <c r="Z36" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>5743</t>
+      <c r="AA36" t="n">
+        <v>5743</v>
+      </c>
+      <c r="AB36" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>6353</t>
         </is>
       </c>
     </row>
@@ -3771,9 +3987,15 @@
       <c r="Z37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>5627</t>
+      <c r="AA37" t="n">
+        <v>5627</v>
+      </c>
+      <c r="AB37" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>6000</t>
         </is>
       </c>
     </row>
@@ -3862,9 +4084,15 @@
       <c r="Z38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>5664</t>
+      <c r="AA38" t="n">
+        <v>5664</v>
+      </c>
+      <c r="AB38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>6115</t>
         </is>
       </c>
     </row>
@@ -3953,9 +4181,15 @@
       <c r="Z39" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA39" t="inlineStr">
-        <is>
-          <t>5905</t>
+      <c r="AA39" t="n">
+        <v>5905</v>
+      </c>
+      <c r="AB39" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>6280</t>
         </is>
       </c>
     </row>
@@ -3978,7 +4212,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F40" s="5" t="n">
@@ -4044,9 +4278,15 @@
       <c r="Z40" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AA40" t="inlineStr">
-        <is>
-          <t>6255</t>
+      <c r="AA40" t="n">
+        <v>6255</v>
+      </c>
+      <c r="AB40" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>6818</t>
         </is>
       </c>
     </row>
@@ -4135,9 +4375,15 @@
       <c r="Z41" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>5839</t>
+      <c r="AA41" t="n">
+        <v>5839</v>
+      </c>
+      <c r="AB41" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>6227</t>
         </is>
       </c>
     </row>
@@ -4226,9 +4472,15 @@
       <c r="Z42" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>4856</t>
+      <c r="AA42" t="n">
+        <v>4856</v>
+      </c>
+      <c r="AB42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>5107</t>
         </is>
       </c>
     </row>
@@ -4317,9 +4569,15 @@
       <c r="Z43" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AA43" t="inlineStr">
-        <is>
-          <t>5803</t>
+      <c r="AA43" t="n">
+        <v>5803</v>
+      </c>
+      <c r="AB43" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>6471</t>
         </is>
       </c>
     </row>
@@ -4408,9 +4666,15 @@
       <c r="Z44" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>5668</t>
+      <c r="AA44" t="n">
+        <v>5668</v>
+      </c>
+      <c r="AB44" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>6174</t>
         </is>
       </c>
     </row>
@@ -4499,9 +4763,15 @@
       <c r="Z45" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t>5188</t>
+      <c r="AA45" t="n">
+        <v>5188</v>
+      </c>
+      <c r="AB45" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>5437</t>
         </is>
       </c>
     </row>
@@ -4590,9 +4860,15 @@
       <c r="Z46" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>5452</t>
+      <c r="AA46" t="n">
+        <v>5452</v>
+      </c>
+      <c r="AB46" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>5908</t>
         </is>
       </c>
     </row>
@@ -4681,9 +4957,15 @@
       <c r="Z47" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AA47" t="inlineStr">
-        <is>
-          <t>4988</t>
+      <c r="AA47" t="n">
+        <v>4988</v>
+      </c>
+      <c r="AB47" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>5253</t>
         </is>
       </c>
     </row>
@@ -4772,9 +5054,15 @@
       <c r="Z48" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA48" t="inlineStr">
-        <is>
-          <t>5685</t>
+      <c r="AA48" t="n">
+        <v>5685</v>
+      </c>
+      <c r="AB48" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>5935</t>
         </is>
       </c>
     </row>
@@ -4797,7 +5085,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F49" s="5" t="n">
@@ -4863,9 +5151,15 @@
       <c r="Z49" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>5242</t>
+      <c r="AA49" t="n">
+        <v>5242</v>
+      </c>
+      <c r="AB49" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>6012</t>
         </is>
       </c>
     </row>
@@ -4954,9 +5248,15 @@
       <c r="Z50" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA50" t="inlineStr">
-        <is>
-          <t>3169</t>
+      <c r="AA50" t="n">
+        <v>3169</v>
+      </c>
+      <c r="AB50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>3225</t>
         </is>
       </c>
     </row>
@@ -5045,9 +5345,15 @@
       <c r="Z51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>3302</t>
+      <c r="AA51" t="n">
+        <v>3302</v>
+      </c>
+      <c r="AB51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>3656</t>
         </is>
       </c>
     </row>
@@ -5136,9 +5442,15 @@
       <c r="Z52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA52" t="inlineStr">
-        <is>
-          <t>4456</t>
+      <c r="AA52" t="n">
+        <v>4456</v>
+      </c>
+      <c r="AB52" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>4852</t>
         </is>
       </c>
     </row>
@@ -5227,9 +5539,15 @@
       <c r="Z53" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA53" t="inlineStr">
-        <is>
-          <t>4256</t>
+      <c r="AA53" t="n">
+        <v>4256</v>
+      </c>
+      <c r="AB53" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>4405</t>
         </is>
       </c>
     </row>
@@ -5318,9 +5636,15 @@
       <c r="Z54" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA54" t="inlineStr">
-        <is>
-          <t>4474</t>
+      <c r="AA54" t="n">
+        <v>4474</v>
+      </c>
+      <c r="AB54" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>4717</t>
         </is>
       </c>
     </row>
@@ -5404,6 +5728,8 @@
       <c r="Y55" t="inlineStr"/>
       <c r="Z55" s="3" t="inlineStr"/>
       <c r="AA55" t="inlineStr"/>
+      <c r="AB55" s="3" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -5490,9 +5816,15 @@
       <c r="Z56" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>5210</t>
+      <c r="AA56" t="n">
+        <v>5210</v>
+      </c>
+      <c r="AB56" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>5571</t>
         </is>
       </c>
     </row>
@@ -5581,9 +5913,15 @@
       <c r="Z57" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>4325</t>
+      <c r="AA57" t="n">
+        <v>4325</v>
+      </c>
+      <c r="AB57" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>4704</t>
         </is>
       </c>
     </row>
@@ -5672,9 +6010,15 @@
       <c r="Z58" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>5158</t>
+      <c r="AA58" t="n">
+        <v>5158</v>
+      </c>
+      <c r="AB58" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>5344</t>
         </is>
       </c>
     </row>
@@ -5763,9 +6107,15 @@
       <c r="Z59" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AA59" t="inlineStr">
-        <is>
-          <t>5286</t>
+      <c r="AA59" t="n">
+        <v>5286</v>
+      </c>
+      <c r="AB59" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>5727</t>
         </is>
       </c>
     </row>
@@ -5854,9 +6204,15 @@
       <c r="Z60" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>5065</t>
+      <c r="AA60" t="n">
+        <v>5065</v>
+      </c>
+      <c r="AB60" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>5423</t>
         </is>
       </c>
     </row>
@@ -5879,7 +6235,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F61" s="5" t="n">
@@ -5945,9 +6301,15 @@
       <c r="Z61" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AA61" t="inlineStr">
-        <is>
-          <t>6889</t>
+      <c r="AA61" t="n">
+        <v>6889</v>
+      </c>
+      <c r="AB61" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>7117</t>
         </is>
       </c>
     </row>
@@ -6036,9 +6398,15 @@
       <c r="Z62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA62" t="inlineStr">
-        <is>
-          <t>5126</t>
+      <c r="AA62" t="n">
+        <v>5126</v>
+      </c>
+      <c r="AB62" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>5564</t>
         </is>
       </c>
     </row>
@@ -6127,9 +6495,15 @@
       <c r="Z63" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>4477</t>
+      <c r="AA63" t="n">
+        <v>4477</v>
+      </c>
+      <c r="AB63" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>4648</t>
         </is>
       </c>
     </row>
@@ -6218,9 +6592,15 @@
       <c r="Z64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA64" t="inlineStr">
-        <is>
-          <t>4204</t>
+      <c r="AA64" t="n">
+        <v>4204</v>
+      </c>
+      <c r="AB64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC64" t="inlineStr">
+        <is>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -6309,9 +6689,15 @@
       <c r="Z65" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AA65" t="inlineStr">
-        <is>
-          <t>4497</t>
+      <c r="AA65" t="n">
+        <v>4497</v>
+      </c>
+      <c r="AB65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC65" t="inlineStr">
+        <is>
+          <t>4676</t>
         </is>
       </c>
     </row>
@@ -6400,9 +6786,15 @@
       <c r="Z66" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AA66" t="inlineStr">
-        <is>
-          <t>5177</t>
+      <c r="AA66" t="n">
+        <v>5177</v>
+      </c>
+      <c r="AB66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC66" t="inlineStr">
+        <is>
+          <t>5457</t>
         </is>
       </c>
     </row>
@@ -6491,9 +6883,15 @@
       <c r="Z67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA67" t="inlineStr">
-        <is>
-          <t>4478</t>
+      <c r="AA67" t="n">
+        <v>4478</v>
+      </c>
+      <c r="AB67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC67" t="inlineStr">
+        <is>
+          <t>4649</t>
         </is>
       </c>
     </row>
@@ -6582,9 +6980,15 @@
       <c r="Z68" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA68" t="inlineStr">
-        <is>
-          <t>3860</t>
+      <c r="AA68" t="n">
+        <v>3860</v>
+      </c>
+      <c r="AB68" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC68" t="inlineStr">
+        <is>
+          <t>4537</t>
         </is>
       </c>
     </row>
@@ -6673,9 +7077,15 @@
       <c r="Z69" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>3845</t>
+      <c r="AA69" t="n">
+        <v>3845</v>
+      </c>
+      <c r="AB69" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>3926</t>
         </is>
       </c>
     </row>
@@ -6764,9 +7174,15 @@
       <c r="Z70" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA70" t="inlineStr">
-        <is>
-          <t>5637</t>
+      <c r="AA70" t="n">
+        <v>5637</v>
+      </c>
+      <c r="AB70" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC70" t="inlineStr">
+        <is>
+          <t>5911</t>
         </is>
       </c>
     </row>
@@ -6855,9 +7271,15 @@
       <c r="Z71" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AA71" t="inlineStr">
-        <is>
-          <t>5372</t>
+      <c r="AA71" t="n">
+        <v>5372</v>
+      </c>
+      <c r="AB71" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC71" t="inlineStr">
+        <is>
+          <t>6108</t>
         </is>
       </c>
     </row>
@@ -6946,9 +7368,15 @@
       <c r="Z72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA72" t="inlineStr">
-        <is>
-          <t>4544</t>
+      <c r="AA72" t="n">
+        <v>4544</v>
+      </c>
+      <c r="AB72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC72" t="inlineStr">
+        <is>
+          <t>4782</t>
         </is>
       </c>
     </row>
@@ -7037,9 +7465,15 @@
       <c r="Z73" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA73" t="inlineStr">
-        <is>
-          <t>5068</t>
+      <c r="AA73" t="n">
+        <v>5068</v>
+      </c>
+      <c r="AB73" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC73" t="inlineStr">
+        <is>
+          <t>5393</t>
         </is>
       </c>
     </row>
@@ -7095,6 +7529,8 @@
       <c r="Y74" t="inlineStr"/>
       <c r="Z74" s="3" t="inlineStr"/>
       <c r="AA74" t="inlineStr"/>
+      <c r="AB74" s="3" t="inlineStr"/>
+      <c r="AC74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -7181,9 +7617,15 @@
       <c r="Z75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA75" t="inlineStr">
-        <is>
-          <t>4757</t>
+      <c r="AA75" t="n">
+        <v>4757</v>
+      </c>
+      <c r="AB75" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC75" t="inlineStr">
+        <is>
+          <t>5055</t>
         </is>
       </c>
     </row>
@@ -7272,9 +7714,15 @@
       <c r="Z76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA76" t="inlineStr">
-        <is>
-          <t>4753</t>
+      <c r="AA76" t="n">
+        <v>4753</v>
+      </c>
+      <c r="AB76" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>4926</t>
         </is>
       </c>
     </row>
@@ -7363,9 +7811,15 @@
       <c r="Z77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA77" t="inlineStr">
-        <is>
-          <t>4492</t>
+      <c r="AA77" t="n">
+        <v>4492</v>
+      </c>
+      <c r="AB77" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC77" t="inlineStr">
+        <is>
+          <t>4736</t>
         </is>
       </c>
     </row>
@@ -7454,9 +7908,15 @@
       <c r="Z78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA78" t="inlineStr">
-        <is>
-          <t>3874</t>
+      <c r="AA78" t="n">
+        <v>3874</v>
+      </c>
+      <c r="AB78" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC78" t="inlineStr">
+        <is>
+          <t>3914</t>
         </is>
       </c>
     </row>
@@ -7545,9 +8005,15 @@
       <c r="Z79" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA79" t="inlineStr">
-        <is>
-          <t>3643</t>
+      <c r="AA79" t="n">
+        <v>3643</v>
+      </c>
+      <c r="AB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC79" t="inlineStr">
+        <is>
+          <t>3754</t>
         </is>
       </c>
     </row>
@@ -7636,9 +8102,15 @@
       <c r="Z80" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AA80" t="inlineStr">
-        <is>
-          <t>4791</t>
+      <c r="AA80" t="n">
+        <v>4791</v>
+      </c>
+      <c r="AB80" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>5001</t>
         </is>
       </c>
     </row>
@@ -7727,9 +8199,15 @@
       <c r="Z81" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA81" t="inlineStr">
-        <is>
-          <t>2754</t>
+      <c r="AA81" t="n">
+        <v>2754</v>
+      </c>
+      <c r="AB81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC81" t="inlineStr">
+        <is>
+          <t>2886</t>
         </is>
       </c>
     </row>
@@ -7818,9 +8296,15 @@
       <c r="Z82" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA82" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="AA82" t="n">
+        <v>3369</v>
+      </c>
+      <c r="AB82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC82" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -7901,11 +8385,11 @@
       <c r="Z83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA83" t="inlineStr">
-        <is>
-          <t>2327</t>
-        </is>
-      </c>
+      <c r="AA83" t="n">
+        <v>2327</v>
+      </c>
+      <c r="AB83" s="3" t="inlineStr"/>
+      <c r="AC83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -7992,9 +8476,15 @@
       <c r="Z84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA84" t="inlineStr">
-        <is>
-          <t>2259</t>
+      <c r="AA84" t="n">
+        <v>2259</v>
+      </c>
+      <c r="AB84" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC84" t="inlineStr">
+        <is>
+          <t>2289</t>
         </is>
       </c>
     </row>
@@ -8038,6 +8528,8 @@
       <c r="Y85" t="inlineStr"/>
       <c r="Z85" s="3" t="inlineStr"/>
       <c r="AA85" t="inlineStr"/>
+      <c r="AB85" s="3" t="inlineStr"/>
+      <c r="AC85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -8124,9 +8616,15 @@
       <c r="Z86" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA86" t="inlineStr">
-        <is>
-          <t>2586</t>
+      <c r="AA86" t="n">
+        <v>2586</v>
+      </c>
+      <c r="AB86" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC86" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -8215,9 +8713,15 @@
       <c r="Z87" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA87" t="inlineStr">
-        <is>
-          <t>3337</t>
+      <c r="AA87" t="n">
+        <v>3337</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" t="inlineStr">
+        <is>
+          <t>3488</t>
         </is>
       </c>
     </row>
@@ -8273,6 +8777,8 @@
       <c r="Y88" t="inlineStr"/>
       <c r="Z88" s="3" t="inlineStr"/>
       <c r="AA88" t="inlineStr"/>
+      <c r="AB88" s="3" t="inlineStr"/>
+      <c r="AC88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -8359,9 +8865,15 @@
       <c r="Z89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA89" t="inlineStr">
-        <is>
-          <t>2342</t>
+      <c r="AA89" t="n">
+        <v>2342</v>
+      </c>
+      <c r="AB89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC89" t="inlineStr">
+        <is>
+          <t>2317</t>
         </is>
       </c>
     </row>
@@ -8450,9 +8962,15 @@
       <c r="Z90" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA90" t="inlineStr">
-        <is>
-          <t>3005</t>
+      <c r="AA90" t="n">
+        <v>3005</v>
+      </c>
+      <c r="AB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC90" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -8541,9 +9059,15 @@
       <c r="Z91" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA91" t="inlineStr">
-        <is>
-          <t>3480</t>
+      <c r="AA91" t="n">
+        <v>3480</v>
+      </c>
+      <c r="AB91" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC91" t="inlineStr">
+        <is>
+          <t>4103</t>
         </is>
       </c>
     </row>
@@ -8632,9 +9156,15 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="AA92" t="n">
+        <v>3369</v>
+      </c>
+      <c r="AB92" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC92" t="inlineStr">
+        <is>
+          <t>3655</t>
         </is>
       </c>
     </row>
@@ -8723,9 +9253,15 @@
       <c r="Z93" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA93" t="inlineStr">
-        <is>
-          <t>4420</t>
+      <c r="AA93" t="n">
+        <v>4420</v>
+      </c>
+      <c r="AB93" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC93" t="inlineStr">
+        <is>
+          <t>4592</t>
         </is>
       </c>
     </row>
@@ -8814,9 +9350,15 @@
       <c r="Z94" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA94" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="AA94" t="n">
+        <v>4172</v>
+      </c>
+      <c r="AB94" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC94" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -8905,9 +9447,15 @@
       <c r="Z95" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AA95" t="inlineStr">
-        <is>
-          <t>4118</t>
+      <c r="AA95" t="n">
+        <v>4118</v>
+      </c>
+      <c r="AB95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC95" t="inlineStr">
+        <is>
+          <t>4325</t>
         </is>
       </c>
     </row>
@@ -8996,9 +9544,15 @@
       <c r="Z96" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AA96" t="inlineStr">
-        <is>
-          <t>4658</t>
+      <c r="AA96" t="n">
+        <v>4658</v>
+      </c>
+      <c r="AB96" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC96" t="inlineStr">
+        <is>
+          <t>4845</t>
         </is>
       </c>
     </row>
@@ -9054,6 +9608,8 @@
       <c r="Y97" t="inlineStr"/>
       <c r="Z97" s="3" t="inlineStr"/>
       <c r="AA97" t="inlineStr"/>
+      <c r="AB97" s="3" t="inlineStr"/>
+      <c r="AC97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -9140,9 +9696,15 @@
       <c r="Z98" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA98" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="AA98" t="n">
+        <v>2923</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
+        <is>
+          <t>3019</t>
         </is>
       </c>
     </row>
@@ -9231,9 +9793,15 @@
       <c r="Z99" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA99" t="inlineStr">
-        <is>
-          <t>4045</t>
+      <c r="AA99" t="n">
+        <v>4045</v>
+      </c>
+      <c r="AB99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC99" t="inlineStr">
+        <is>
+          <t>4116</t>
         </is>
       </c>
     </row>
@@ -9322,9 +9890,15 @@
       <c r="Z100" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA100" t="inlineStr">
-        <is>
-          <t>3642</t>
+      <c r="AA100" t="n">
+        <v>3642</v>
+      </c>
+      <c r="AB100" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC100" t="inlineStr">
+        <is>
+          <t>3800</t>
         </is>
       </c>
     </row>
@@ -9413,9 +9987,15 @@
       <c r="Z101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA101" t="inlineStr">
-        <is>
-          <t>2678</t>
+      <c r="AA101" t="n">
+        <v>2678</v>
+      </c>
+      <c r="AB101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC101" t="inlineStr">
+        <is>
+          <t>2753</t>
         </is>
       </c>
     </row>
@@ -9504,9 +10084,15 @@
       <c r="Z102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA102" t="inlineStr">
-        <is>
-          <t>2727</t>
+      <c r="AA102" t="n">
+        <v>2727</v>
+      </c>
+      <c r="AB102" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC102" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -9595,9 +10181,15 @@
       <c r="Z103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA103" t="inlineStr">
-        <is>
-          <t>3404</t>
+      <c r="AA103" t="n">
+        <v>3404</v>
+      </c>
+      <c r="AB103" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC103" t="inlineStr">
+        <is>
+          <t>3584</t>
         </is>
       </c>
     </row>
@@ -9686,9 +10278,15 @@
       <c r="Z104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA104" t="inlineStr">
-        <is>
-          <t>3808</t>
+      <c r="AA104" t="n">
+        <v>3808</v>
+      </c>
+      <c r="AB104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC104" t="inlineStr">
+        <is>
+          <t>4004</t>
         </is>
       </c>
     </row>
@@ -9744,6 +10342,8 @@
       <c r="Y105" t="inlineStr"/>
       <c r="Z105" s="3" t="inlineStr"/>
       <c r="AA105" t="inlineStr"/>
+      <c r="AB105" s="3" t="inlineStr"/>
+      <c r="AC105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9785,6 +10385,8 @@
       <c r="Y106" t="inlineStr"/>
       <c r="Z106" s="3" t="inlineStr"/>
       <c r="AA106" t="inlineStr"/>
+      <c r="AB106" s="3" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9854,6 +10456,8 @@
       <c r="Y107" t="inlineStr"/>
       <c r="Z107" s="3" t="inlineStr"/>
       <c r="AA107" t="inlineStr"/>
+      <c r="AB107" s="3" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9940,9 +10544,15 @@
       <c r="Z108" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA108" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="AA108" t="n">
+        <v>2804</v>
+      </c>
+      <c r="AB108" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC108" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -10031,9 +10641,15 @@
       <c r="Z109" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA109" t="inlineStr">
-        <is>
-          <t>3589</t>
+      <c r="AA109" t="n">
+        <v>3589</v>
+      </c>
+      <c r="AB109" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC109" t="inlineStr">
+        <is>
+          <t>3782</t>
         </is>
       </c>
     </row>
@@ -10122,9 +10738,15 @@
       <c r="Z110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA110" t="inlineStr">
-        <is>
-          <t>3469</t>
+      <c r="AA110" t="n">
+        <v>3469</v>
+      </c>
+      <c r="AB110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC110" t="inlineStr">
+        <is>
+          <t>3565</t>
         </is>
       </c>
     </row>
@@ -10213,9 +10835,15 @@
       <c r="Z111" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="AA111" t="inlineStr">
-        <is>
-          <t>4451</t>
+      <c r="AA111" t="n">
+        <v>4451</v>
+      </c>
+      <c r="AB111" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC111" t="inlineStr">
+        <is>
+          <t>4771</t>
         </is>
       </c>
     </row>
@@ -10304,9 +10932,15 @@
       <c r="Z112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA112" t="inlineStr">
-        <is>
-          <t>3499</t>
+      <c r="AA112" t="n">
+        <v>3499</v>
+      </c>
+      <c r="AB112" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC112" t="inlineStr">
+        <is>
+          <t>3681</t>
         </is>
       </c>
     </row>
@@ -10395,9 +11029,15 @@
       <c r="Z113" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>4585</t>
+      <c r="AA113" t="n">
+        <v>4585</v>
+      </c>
+      <c r="AB113" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC113" t="inlineStr">
+        <is>
+          <t>4717</t>
         </is>
       </c>
     </row>
@@ -10486,9 +11126,15 @@
       <c r="Z114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA114" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="AA114" t="n">
+        <v>3159</v>
+      </c>
+      <c r="AB114" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC114" t="inlineStr">
+        <is>
+          <t>3325</t>
         </is>
       </c>
     </row>
@@ -10577,9 +11223,15 @@
       <c r="Z115" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>3706</t>
+      <c r="AA115" t="n">
+        <v>3706</v>
+      </c>
+      <c r="AB115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>3962</t>
         </is>
       </c>
     </row>
@@ -10668,9 +11320,15 @@
       <c r="Z116" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA116" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="AA116" t="n">
+        <v>3003</v>
+      </c>
+      <c r="AB116" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC116" t="inlineStr">
+        <is>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -10759,9 +11417,15 @@
       <c r="Z117" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>3091</t>
+      <c r="AA117" t="n">
+        <v>3091</v>
+      </c>
+      <c r="AB117" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC117" t="inlineStr">
+        <is>
+          <t>3234</t>
         </is>
       </c>
     </row>
@@ -10850,9 +11514,15 @@
       <c r="Z118" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA118" t="inlineStr">
-        <is>
-          <t>3350</t>
+      <c r="AA118" t="n">
+        <v>3350</v>
+      </c>
+      <c r="AB118" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC118" t="inlineStr">
+        <is>
+          <t>3443</t>
         </is>
       </c>
     </row>
@@ -10941,9 +11611,15 @@
       <c r="Z119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA119" t="inlineStr">
-        <is>
-          <t>3200</t>
+      <c r="AA119" t="n">
+        <v>3200</v>
+      </c>
+      <c r="AB119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC119" t="inlineStr">
+        <is>
+          <t>3275</t>
         </is>
       </c>
     </row>
@@ -11032,9 +11708,15 @@
       <c r="Z120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA120" t="inlineStr">
-        <is>
-          <t>3456</t>
+      <c r="AA120" t="n">
+        <v>3456</v>
+      </c>
+      <c r="AB120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC120" t="inlineStr">
+        <is>
+          <t>3679</t>
         </is>
       </c>
     </row>
@@ -11103,9 +11785,15 @@
       <c r="Z121" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA121" t="inlineStr">
-        <is>
-          <t>3297</t>
+      <c r="AA121" t="n">
+        <v>3297</v>
+      </c>
+      <c r="AB121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC121" t="inlineStr">
+        <is>
+          <t>3350</t>
         </is>
       </c>
     </row>
@@ -11194,9 +11882,15 @@
       <c r="Z122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA122" t="inlineStr">
-        <is>
-          <t>2488</t>
+      <c r="AA122" t="n">
+        <v>2488</v>
+      </c>
+      <c r="AB122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC122" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -11252,6 +11946,8 @@
       <c r="Y123" t="inlineStr"/>
       <c r="Z123" s="3" t="inlineStr"/>
       <c r="AA123" t="inlineStr"/>
+      <c r="AB123" s="3" t="inlineStr"/>
+      <c r="AC123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -11305,6 +12001,8 @@
       <c r="Y124" t="inlineStr"/>
       <c r="Z124" s="3" t="inlineStr"/>
       <c r="AA124" t="inlineStr"/>
+      <c r="AB124" s="3" t="inlineStr"/>
+      <c r="AC124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -11391,9 +12089,15 @@
       <c r="Z125" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AA125" t="inlineStr">
-        <is>
-          <t>2593</t>
+      <c r="AA125" t="n">
+        <v>2593</v>
+      </c>
+      <c r="AB125" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC125" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
@@ -11445,6 +12149,8 @@
       <c r="Y126" t="inlineStr"/>
       <c r="Z126" s="3" t="inlineStr"/>
       <c r="AA126" t="inlineStr"/>
+      <c r="AB126" s="3" t="inlineStr"/>
+      <c r="AC126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -11531,9 +12237,15 @@
       <c r="Z127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA127" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="AA127" t="n">
+        <v>2815</v>
+      </c>
+      <c r="AB127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC127" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -11622,9 +12334,15 @@
       <c r="Z128" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA128" t="inlineStr">
-        <is>
-          <t>3804</t>
+      <c r="AA128" t="n">
+        <v>3804</v>
+      </c>
+      <c r="AB128" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC128" t="inlineStr">
+        <is>
+          <t>3970</t>
         </is>
       </c>
     </row>
@@ -11676,6 +12394,8 @@
       <c r="Y129" t="inlineStr"/>
       <c r="Z129" s="3" t="inlineStr"/>
       <c r="AA129" t="inlineStr"/>
+      <c r="AB129" s="3" t="inlineStr"/>
+      <c r="AC129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -11762,7 +12482,13 @@
       <c r="Z130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA130" t="inlineStr">
+      <c r="AA130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11816,6 +12542,8 @@
       <c r="Y131" t="inlineStr"/>
       <c r="Z131" s="3" t="inlineStr"/>
       <c r="AA131" t="inlineStr"/>
+      <c r="AB131" s="3" t="inlineStr"/>
+      <c r="AC131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -11902,7 +12630,13 @@
       <c r="Z132" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA132" t="inlineStr">
+      <c r="AA132" t="n">
+        <v>2754</v>
+      </c>
+      <c r="AB132" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC132" t="inlineStr">
         <is>
           <t>2754</t>
         </is>
@@ -11993,9 +12727,15 @@
       <c r="Z133" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AA133" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="AA133" t="n">
+        <v>2879</v>
+      </c>
+      <c r="AB133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC133" t="inlineStr">
+        <is>
+          <t>2878</t>
         </is>
       </c>
     </row>
@@ -12047,6 +12787,8 @@
       <c r="Y134" t="inlineStr"/>
       <c r="Z134" s="3" t="inlineStr"/>
       <c r="AA134" t="inlineStr"/>
+      <c r="AB134" s="3" t="inlineStr"/>
+      <c r="AC134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -12096,6 +12838,8 @@
       <c r="Y135" t="inlineStr"/>
       <c r="Z135" s="3" t="inlineStr"/>
       <c r="AA135" t="inlineStr"/>
+      <c r="AB135" s="3" t="inlineStr"/>
+      <c r="AC135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -12182,9 +12926,15 @@
       <c r="Z136" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AA136" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="AA136" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AB136" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC136" t="inlineStr">
+        <is>
+          <t>2657</t>
         </is>
       </c>
     </row>
@@ -12236,6 +12986,8 @@
       <c r="Y137" t="inlineStr"/>
       <c r="Z137" s="3" t="inlineStr"/>
       <c r="AA137" t="inlineStr"/>
+      <c r="AB137" s="3" t="inlineStr"/>
+      <c r="AC137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -12285,6 +13037,8 @@
       <c r="Y138" t="inlineStr"/>
       <c r="Z138" s="3" t="inlineStr"/>
       <c r="AA138" t="inlineStr"/>
+      <c r="AB138" s="3" t="inlineStr"/>
+      <c r="AC138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -12371,9 +13125,15 @@
       <c r="Z139" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AA139" t="inlineStr">
-        <is>
-          <t>2404</t>
+      <c r="AA139" t="n">
+        <v>2404</v>
+      </c>
+      <c r="AB139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC139" t="inlineStr">
+        <is>
+          <t>2427</t>
         </is>
       </c>
     </row>
@@ -12462,9 +13222,15 @@
       <c r="Z140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA140" t="inlineStr">
-        <is>
-          <t>1816</t>
+      <c r="AA140" t="n">
+        <v>1816</v>
+      </c>
+      <c r="AB140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC140" t="inlineStr">
+        <is>
+          <t>1813</t>
         </is>
       </c>
     </row>
@@ -12516,6 +13282,8 @@
       <c r="Y141" t="inlineStr"/>
       <c r="Z141" s="3" t="inlineStr"/>
       <c r="AA141" t="inlineStr"/>
+      <c r="AB141" s="3" t="inlineStr"/>
+      <c r="AC141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -12602,9 +13370,15 @@
       <c r="Z142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA142" t="inlineStr">
-        <is>
-          <t>2160</t>
+      <c r="AA142" t="n">
+        <v>2160</v>
+      </c>
+      <c r="AB142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC142" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12693,9 +13467,15 @@
       <c r="Z143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA143" t="inlineStr">
-        <is>
-          <t>1533</t>
+      <c r="AA143" t="n">
+        <v>1533</v>
+      </c>
+      <c r="AB143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC143" t="inlineStr">
+        <is>
+          <t>1531</t>
         </is>
       </c>
     </row>
@@ -12760,7 +13540,13 @@
       <c r="Z144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA144" t="inlineStr">
+      <c r="AA144" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12814,6 +13600,8 @@
       <c r="Y145" t="inlineStr"/>
       <c r="Z145" s="3" t="inlineStr"/>
       <c r="AA145" t="inlineStr"/>
+      <c r="AB145" s="3" t="inlineStr"/>
+      <c r="AC145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -12900,9 +13688,15 @@
       <c r="Z146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA146" t="inlineStr">
-        <is>
-          <t>2418</t>
+      <c r="AA146" t="n">
+        <v>2418</v>
+      </c>
+      <c r="AB146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC146" t="inlineStr">
+        <is>
+          <t>2409</t>
         </is>
       </c>
     </row>
@@ -12991,9 +13785,15 @@
       <c r="Z147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA147" t="inlineStr">
-        <is>
-          <t>2256</t>
+      <c r="AA147" t="n">
+        <v>2256</v>
+      </c>
+      <c r="AB147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC147" t="inlineStr">
+        <is>
+          <t>2279</t>
         </is>
       </c>
     </row>
@@ -13045,6 +13845,8 @@
       <c r="Y148" t="inlineStr"/>
       <c r="Z148" s="3" t="inlineStr"/>
       <c r="AA148" t="inlineStr"/>
+      <c r="AB148" s="3" t="inlineStr"/>
+      <c r="AC148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -13094,6 +13896,8 @@
       <c r="Y149" t="inlineStr"/>
       <c r="Z149" s="3" t="inlineStr"/>
       <c r="AA149" t="inlineStr"/>
+      <c r="AB149" s="3" t="inlineStr"/>
+      <c r="AC149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -13143,6 +13947,8 @@
       <c r="Y150" t="inlineStr"/>
       <c r="Z150" s="3" t="inlineStr"/>
       <c r="AA150" t="inlineStr"/>
+      <c r="AB150" s="3" t="inlineStr"/>
+      <c r="AC150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -13229,9 +14035,15 @@
       <c r="Z151" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="AA151" t="inlineStr">
-        <is>
-          <t>4949</t>
+      <c r="AA151" t="n">
+        <v>4949</v>
+      </c>
+      <c r="AB151" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC151" t="inlineStr">
+        <is>
+          <t>5578</t>
         </is>
       </c>
     </row>
@@ -13320,7 +14132,13 @@
       <c r="Z152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA152" t="inlineStr">
+      <c r="AA152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13411,9 +14229,15 @@
       <c r="Z153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA153" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="AA153" t="n">
+        <v>2516</v>
+      </c>
+      <c r="AB153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC153" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -13502,9 +14326,15 @@
       <c r="Z154" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AA154" t="inlineStr">
-        <is>
-          <t>4286</t>
+      <c r="AA154" t="n">
+        <v>4286</v>
+      </c>
+      <c r="AB154" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC154" t="inlineStr">
+        <is>
+          <t>4828</t>
         </is>
       </c>
     </row>
@@ -13593,7 +14423,13 @@
       <c r="Z155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA155" t="inlineStr">
+      <c r="AA155" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13684,9 +14520,15 @@
       <c r="Z156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA156" t="inlineStr">
-        <is>
-          <t>2788</t>
+      <c r="AA156" t="n">
+        <v>2788</v>
+      </c>
+      <c r="AB156" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC156" t="inlineStr">
+        <is>
+          <t>3271</t>
         </is>
       </c>
     </row>
@@ -13754,6 +14596,8 @@
       <c r="Y157" t="inlineStr"/>
       <c r="Z157" s="3" t="inlineStr"/>
       <c r="AA157" t="inlineStr"/>
+      <c r="AB157" s="3" t="inlineStr"/>
+      <c r="AC157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -13840,7 +14684,13 @@
       <c r="Z158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA158" t="inlineStr">
+      <c r="AA158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13931,9 +14781,15 @@
       <c r="Z159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA159" t="inlineStr">
-        <is>
-          <t>3235</t>
+      <c r="AA159" t="n">
+        <v>3235</v>
+      </c>
+      <c r="AB159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC159" t="inlineStr">
+        <is>
+          <t>3367</t>
         </is>
       </c>
     </row>
@@ -13943,7 +14799,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>爺玩的就是傳說中的寂寞與悲傷</t>
+          <t>"煙神在此 爾等跪拜 ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -14016,9 +14872,15 @@
       <c r="Z160" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA160" t="inlineStr">
-        <is>
-          <t>6129</t>
+      <c r="AA160" t="n">
+        <v>6129</v>
+      </c>
+      <c r="AB160" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC160" t="inlineStr">
+        <is>
+          <t>6845</t>
         </is>
       </c>
     </row>
@@ -14101,9 +14963,15 @@
       <c r="Z161" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AA161" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="AA161" t="n">
+        <v>2618</v>
+      </c>
+      <c r="AB161" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC161" t="inlineStr">
+        <is>
+          <t>2681</t>
         </is>
       </c>
     </row>
@@ -14149,6 +15017,8 @@
       <c r="Y162" t="inlineStr"/>
       <c r="Z162" s="3" t="inlineStr"/>
       <c r="AA162" t="inlineStr"/>
+      <c r="AB162" s="3" t="inlineStr"/>
+      <c r="AC162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -14204,6 +15074,8 @@
       <c r="Y163" t="inlineStr"/>
       <c r="Z163" s="3" t="inlineStr"/>
       <c r="AA163" t="inlineStr"/>
+      <c r="AB163" s="3" t="inlineStr"/>
+      <c r="AC163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -14268,9 +15140,15 @@
       <c r="Z164" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA164" t="inlineStr">
-        <is>
-          <t>4707</t>
+      <c r="AA164" t="n">
+        <v>4707</v>
+      </c>
+      <c r="AB164" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC164" t="inlineStr">
+        <is>
+          <t>5017</t>
         </is>
       </c>
     </row>
@@ -14337,9 +15215,15 @@
       <c r="Z165" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA165" t="inlineStr">
-        <is>
-          <t>4071</t>
+      <c r="AA165" t="n">
+        <v>4071</v>
+      </c>
+      <c r="AB165" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC165" t="inlineStr">
+        <is>
+          <t>4433</t>
         </is>
       </c>
     </row>
@@ -14402,9 +15286,15 @@
       <c r="Z166" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA166" t="inlineStr">
-        <is>
-          <t>2569</t>
+      <c r="AA166" t="n">
+        <v>2569</v>
+      </c>
+      <c r="AB166" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC166" t="inlineStr">
+        <is>
+          <t>2562</t>
         </is>
       </c>
     </row>
@@ -14450,6 +15340,8 @@
       <c r="Y167" t="inlineStr"/>
       <c r="Z167" s="3" t="inlineStr"/>
       <c r="AA167" t="inlineStr"/>
+      <c r="AB167" s="3" t="inlineStr"/>
+      <c r="AC167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -14510,9 +15402,15 @@
       <c r="Z168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA168" t="inlineStr">
-        <is>
-          <t>1645</t>
+      <c r="AA168" t="n">
+        <v>1645</v>
+      </c>
+      <c r="AB168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC168" t="inlineStr">
+        <is>
+          <t>1637</t>
         </is>
       </c>
     </row>
@@ -14571,9 +15469,15 @@
       <c r="Z169" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA169" t="inlineStr">
-        <is>
-          <t>4071</t>
+      <c r="AA169" t="n">
+        <v>4071</v>
+      </c>
+      <c r="AB169" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC169" t="inlineStr">
+        <is>
+          <t>4458</t>
         </is>
       </c>
     </row>
@@ -14628,9 +15532,15 @@
       <c r="Z170" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA170" t="inlineStr">
-        <is>
-          <t>2067</t>
+      <c r="AA170" t="n">
+        <v>2067</v>
+      </c>
+      <c r="AB170" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC170" t="inlineStr">
+        <is>
+          <t>2050</t>
         </is>
       </c>
     </row>
@@ -14676,6 +15586,8 @@
       <c r="Y171" t="inlineStr"/>
       <c r="Z171" s="3" t="inlineStr"/>
       <c r="AA171" t="inlineStr"/>
+      <c r="AB171" s="3" t="inlineStr"/>
+      <c r="AC171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -14724,9 +15636,15 @@
       <c r="Z172" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="AA172" t="inlineStr">
-        <is>
-          <t>3270</t>
+      <c r="AA172" t="n">
+        <v>3270</v>
+      </c>
+      <c r="AB172" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC172" t="inlineStr">
+        <is>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -14772,6 +15690,8 @@
       <c r="Y173" t="inlineStr"/>
       <c r="Z173" s="3" t="inlineStr"/>
       <c r="AA173" t="inlineStr"/>
+      <c r="AB173" s="3" t="inlineStr"/>
+      <c r="AC173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -14816,9 +15736,15 @@
       <c r="Z174" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA174" t="inlineStr">
-        <is>
-          <t>1092</t>
+      <c r="AA174" t="n">
+        <v>1092</v>
+      </c>
+      <c r="AB174" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC174" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -14861,9 +15787,109 @@
       <c r="Z175" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA175" t="inlineStr">
-        <is>
-          <t>1627</t>
+      <c r="AA175" t="n">
+        <v>1627</v>
+      </c>
+      <c r="AB175" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC175" t="inlineStr">
+        <is>
+          <t>1638</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>43281368</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>xhs2763</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F176" s="3" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" s="3" t="inlineStr"/>
+      <c r="I176" t="inlineStr"/>
+      <c r="J176" s="3" t="inlineStr"/>
+      <c r="K176" t="inlineStr"/>
+      <c r="L176" s="3" t="inlineStr"/>
+      <c r="M176" t="inlineStr"/>
+      <c r="N176" s="3" t="inlineStr"/>
+      <c r="O176" t="inlineStr"/>
+      <c r="P176" s="3" t="inlineStr"/>
+      <c r="Q176" t="inlineStr"/>
+      <c r="R176" s="3" t="inlineStr"/>
+      <c r="S176" t="inlineStr"/>
+      <c r="T176" s="3" t="inlineStr"/>
+      <c r="U176" t="inlineStr"/>
+      <c r="V176" s="3" t="inlineStr"/>
+      <c r="W176" t="inlineStr"/>
+      <c r="X176" s="3" t="inlineStr"/>
+      <c r="Y176" t="inlineStr"/>
+      <c r="Z176" s="3" t="inlineStr"/>
+      <c r="AA176" t="inlineStr"/>
+      <c r="AB176" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC176" t="inlineStr">
+        <is>
+          <t>2959</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>58368224</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>战争雷霆杯</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F177" s="3" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" s="3" t="inlineStr"/>
+      <c r="I177" t="inlineStr"/>
+      <c r="J177" s="3" t="inlineStr"/>
+      <c r="K177" t="inlineStr"/>
+      <c r="L177" s="3" t="inlineStr"/>
+      <c r="M177" t="inlineStr"/>
+      <c r="N177" s="3" t="inlineStr"/>
+      <c r="O177" t="inlineStr"/>
+      <c r="P177" s="3" t="inlineStr"/>
+      <c r="Q177" t="inlineStr"/>
+      <c r="R177" s="3" t="inlineStr"/>
+      <c r="S177" t="inlineStr"/>
+      <c r="T177" s="3" t="inlineStr"/>
+      <c r="U177" t="inlineStr"/>
+      <c r="V177" s="3" t="inlineStr"/>
+      <c r="W177" t="inlineStr"/>
+      <c r="X177" s="3" t="inlineStr"/>
+      <c r="Y177" t="inlineStr"/>
+      <c r="Z177" s="3" t="inlineStr"/>
+      <c r="AA177" t="inlineStr"/>
+      <c r="AB177" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC177" t="inlineStr">
+        <is>
+          <t>1440</t>
         </is>
       </c>
     </row>

</xml_diff>